<commit_message>
working on results and discussion
</commit_message>
<xml_diff>
--- a/Thesis/Resources/CGPerformance.xlsx
+++ b/Thesis/Resources/CGPerformance.xlsx
@@ -5,11 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Memory" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Delta performance" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Laptop performance" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="GRID performance" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="137">
   <si>
     <t xml:space="preserve">3D Parallel 1000</t>
   </si>
@@ -356,7 +359,82 @@
     <t xml:space="preserve">Error</t>
   </si>
   <si>
+    <t xml:space="preserve">3D 64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Double</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single</t>
+  </si>
+  <si>
     <t xml:space="preserve">mesured</t>
+  </si>
+  <si>
+    <t xml:space="preserve">measured</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3D 128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2D Square128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No of iterations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Double precision </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single precision </t>
+  </si>
+  <si>
+    <t xml:space="preserve">New distrib function, version 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New distrib function, version 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Runtime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MLUPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Old distrib function, version 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New distrib function, version 3 (unrolled)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Old distrib function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New distrib function, version 3 (unrolled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final version, arch 50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final version, high order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIVERGENCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final version, arch 35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3D Cube64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3D Cube128</t>
   </si>
 </sst>
 </file>
@@ -366,11 +444,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -392,14 +471,28 @@
       <color rgb="FF000000"/>
       <name val="Monospace"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -408,6 +501,21 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF212121"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -625,7 +733,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -634,111 +742,127 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -808,317 +932,13 @@
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="FF212121"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Color Gradient over 10000 iterations</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$42</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>3D</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$42</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>22.1780798206029</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$65</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>2D</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ff420e"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$65</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>19.4821440632257</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:gapWidth val="100"/>
-        <c:overlap val="0"/>
-        <c:axId val="36788571"/>
-        <c:axId val="65080269"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="36788571"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="65080269"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="65080269"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>MLUPs</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="36788571"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1235,6 +1055,7 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1243,6 +1064,7 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
+              <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1251,6 +1073,7 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
+              <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1259,6 +1082,7 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
+              <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1267,12 +1091,14 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
+              <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
             </c:dLbl>
+            <c:dLblPos val="bestFit"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1350,6 +1176,7 @@
       </c:spPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1362,7 +1189,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1435,6 +1262,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1479,6 +1307,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1501,11 +1330,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="49416845"/>
-        <c:axId val="319794"/>
+        <c:axId val="58512202"/>
+        <c:axId val="39121084"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="49416845"/>
+        <c:axId val="58512202"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1549,14 +1378,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="319794"/>
+        <c:crossAx val="39121084"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="319794"/>
+        <c:axId val="39121084"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1618,7 +1447,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1647,7 +1476,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49416845"/>
+        <c:crossAx val="58512202"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1684,7 +1513,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1757,6 +1586,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1801,6 +1631,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1823,11 +1654,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="2573117"/>
-        <c:axId val="63109459"/>
+        <c:axId val="60212111"/>
+        <c:axId val="97322992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2573117"/>
+        <c:axId val="60212111"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1862,14 +1693,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63109459"/>
+        <c:crossAx val="97322992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63109459"/>
+        <c:axId val="97322992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1922,7 +1753,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1951,7 +1782,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2573117"/>
+        <c:crossAx val="60212111"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1988,7 +1819,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2038,10 +1869,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.194798699674919"/>
-          <c:y val="0.147013102376194"/>
-          <c:w val="0.532070517629407"/>
-          <c:h val="0.829669109482567"/>
+          <c:x val="0.194767932489451"/>
+          <c:y val="0.14704901633878"/>
+          <c:w val="0.531898734177215"/>
+          <c:h val="0.829276425475158"/>
         </c:manualLayout>
       </c:layout>
       <c:pieChart>
@@ -2116,6 +1947,7 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -2124,6 +1956,7 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
+              <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -2132,6 +1965,7 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
+              <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -2140,6 +1974,7 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
+              <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -2148,12 +1983,14 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
+              <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
             </c:dLbl>
+            <c:dLblPos val="bestFit"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -2231,6 +2068,313 @@
       </c:spPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Color Gradient over 10000 iterations</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$42</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3D</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>22.1780798206029</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$65</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2D</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$65</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>19.4821440632257</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:overlap val="0"/>
+        <c:axId val="24343379"/>
+        <c:axId val="78668940"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="24343379"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="78668940"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="78668940"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>MLUPs</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="24343379"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2248,15 +2392,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>521640</xdr:colOff>
+      <xdr:colOff>524520</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>124560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>438480</xdr:colOff>
+      <xdr:colOff>437400</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>95760</xdr:rowOff>
+      <xdr:rowOff>94680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2264,8 +2408,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8494560" y="124560"/>
-        <a:ext cx="5838120" cy="3222360"/>
+        <a:off x="6915600" y="124560"/>
+        <a:ext cx="5389920" cy="3221280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2278,15 +2422,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>438480</xdr:colOff>
+      <xdr:colOff>441360</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>2880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1227240</xdr:colOff>
+      <xdr:colOff>1226880</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>151200</xdr:rowOff>
+      <xdr:rowOff>150120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2294,8 +2438,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6785640" y="4876560"/>
-        <a:ext cx="4680000" cy="3240000"/>
+        <a:off x="5632200" y="4879440"/>
+        <a:ext cx="4138560" cy="3236040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2314,9 +2458,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>338400</xdr:colOff>
+      <xdr:colOff>337320</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>75240</xdr:rowOff>
+      <xdr:rowOff>74160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2324,8 +2468,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9552600" y="8376840"/>
-        <a:ext cx="4680000" cy="3240000"/>
+        <a:off x="7913160" y="8376840"/>
+        <a:ext cx="4292280" cy="3238920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2338,15 +2482,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>129960</xdr:colOff>
+      <xdr:colOff>132840</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>114840</xdr:rowOff>
+      <xdr:rowOff>117720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>198720</xdr:colOff>
+      <xdr:colOff>197640</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>105480</xdr:rowOff>
+      <xdr:rowOff>105120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2354,8 +2498,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="14837040" y="277200"/>
-        <a:ext cx="5758200" cy="3241800"/>
+        <a:off x="12600720" y="280080"/>
+        <a:ext cx="4265640" cy="3238560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2374,9 +2518,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>690840</xdr:colOff>
+      <xdr:colOff>690480</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>17640</xdr:rowOff>
+      <xdr:rowOff>16560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2384,8 +2528,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3983760" y="8319240"/>
-        <a:ext cx="4680000" cy="3240000"/>
+        <a:off x="3465720" y="8319240"/>
+        <a:ext cx="3615840" cy="3238920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2405,22 +2549,22 @@
   </sheetPr>
   <dimension ref="A1:R81"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="O34" activeCellId="0" sqref="O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4744897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.8877551020408"/>
-    <col collapsed="false" hidden="false" max="9" min="5" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.1275510204082"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.9795918367347"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.219387755102"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.0663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="9" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3199,15 +3343,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S51"/>
+  <dimension ref="A1:W54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V54" activeCellId="0" sqref="V54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.5204081632653"/>
+    <col collapsed="false" hidden="false" max="20" min="11" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="12.8061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5178,24 +5326,67 @@
       <c r="Q50" s="27" t="s">
         <v>27</v>
       </c>
+      <c r="U50" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="V50" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="W50" s="28" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E51" s="0" t="n">
         <v>500</v>
       </c>
-      <c r="G51" s="28" t="s">
-        <v>111</v>
-      </c>
-      <c r="I51" s="28" t="n">
+      <c r="G51" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="I51" s="29" t="n">
         <f aca="false">I50+E51</f>
         <v>521.814270019531</v>
       </c>
-      <c r="N51" s="28" t="s">
-        <v>111</v>
-      </c>
-      <c r="P51" s="28" t="n">
+      <c r="N51" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="P51" s="29" t="n">
         <f aca="false">P50+E51</f>
         <v>533.615051269531</v>
+      </c>
+      <c r="U51" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="V51" s="0" t="n">
+        <v>863</v>
+      </c>
+      <c r="W51" s="0" t="n">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U52" s="28"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U53" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="V53" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="W53" s="28" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U54" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="V54" s="0" t="n">
+        <v>3209</v>
+      </c>
+      <c r="W54" s="0" t="n">
+        <v>1708</v>
       </c>
     </row>
   </sheetData>
@@ -5208,7 +5399,1935 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.7040816326531"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <f aca="false">128*128</f>
+        <v>16384</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="F4" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" s="31"/>
+      <c r="F5" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="I5" s="31"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>18.67</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>20.01</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>18.08</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>17.33</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <f aca="false">$A$3*$B$3/B6/1000000</f>
+        <v>8.77557579003749</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <f aca="false">$A$3*$B$3/D6/1000000</f>
+        <v>8.18790604697651</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <f aca="false">$A$3*$B$3/G6/1000000</f>
+        <v>9.06194690265487</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <f aca="false">$A$3*$B$3/I6/1000000</f>
+        <v>9.45412579342181</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="D8" s="31"/>
+      <c r="F8" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="I8" s="31"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>17.99</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>18.13</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>17.860001</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>18.67</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <f aca="false">$A$3*$B$3/B9/1000000</f>
+        <v>9.10728182323513</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <f aca="false">$A$3*$B$3/D9/1000000</f>
+        <v>9.03695532266961</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <f aca="false">$A$3*$B$3/G9/1000000</f>
+        <v>9.17357171480561</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <f aca="false">$A$3*$B$3/I9/1000000</f>
+        <v>8.77557579003749</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:K24"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H22" activeCellId="0" sqref="H22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.0612244897959"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <f aca="false">128*128</f>
+        <v>16384</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="H4" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="D5" s="30"/>
+      <c r="H5" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="K5" s="30"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>20.38836</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>18.081086</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>12.156735</v>
+      </c>
+      <c r="J6" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>10.550231</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <f aca="false">$A$3*$B$3/B6/1000000</f>
+        <v>8.03595777198362</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>17.926045</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <f aca="false">$A$3*$B$3/I6/1000000</f>
+        <v>13.4773029106911</v>
+      </c>
+      <c r="J7" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>9.936819</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>0.008062</v>
+      </c>
+      <c r="J8" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>0.006028</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" s="30"/>
+      <c r="C9" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>6.429288</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="I9" s="30"/>
+      <c r="J9" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>1.882581</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>21.001033</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>1.809068</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>11.087945</v>
+      </c>
+      <c r="J10" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>1.009695</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <f aca="false">$A$3*$B$3/B10/1000000</f>
+        <v>7.8015210013717</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>0.315806</v>
+      </c>
+      <c r="H11" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <f aca="false">$A$3*$B$3/I10/1000000</f>
+        <v>14.7764080720097</v>
+      </c>
+      <c r="J11" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>0.291298</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>3.876738</v>
+      </c>
+      <c r="J12" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>2.031182</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="B13" s="30"/>
+      <c r="C13" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>4.176064</v>
+      </c>
+      <c r="H13" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="I13" s="30"/>
+      <c r="J13" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>3.928059</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>19.937009</v>
+      </c>
+      <c r="C14" s="28"/>
+      <c r="H14" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>10.30279</v>
+      </c>
+      <c r="J14" s="28"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <f aca="false">$A$3*$B$3/B14/1000000</f>
+        <v>8.21788263224439</v>
+      </c>
+      <c r="H15" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <f aca="false">$A$3*$B$3/I14/1000000</f>
+        <v>15.9024885492182</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="B17" s="30"/>
+      <c r="H17" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="I17" s="30"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>21.364202</v>
+      </c>
+      <c r="H18" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>11.187888</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <f aca="false">$A$3*$B$3/B18/1000000</f>
+        <v>7.66890333652528</v>
+      </c>
+      <c r="H19" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <f aca="false">$A$3*$B$3/I18/1000000</f>
+        <v>14.6444083101297</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="D21" s="30"/>
+      <c r="H21" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="K21" s="30"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>18.386505</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="32" t="n">
+        <v>24.130116</v>
+      </c>
+      <c r="H22" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>10.115005</v>
+      </c>
+      <c r="J22" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="K22" s="0" t="n">
+        <v>10.373061</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>18.24269</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>13.207736</v>
+      </c>
+      <c r="H23" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>9.971847</v>
+      </c>
+      <c r="J23" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="K23" s="0" t="n">
+        <v>2.45075</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <f aca="false">$A$3*$B$3/B22/1000000</f>
+        <v>8.91088328097156</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <f aca="false">$A$3*$B$3/D22/1000000</f>
+        <v>6.78985546526175</v>
+      </c>
+      <c r="H24" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <f aca="false">$A$3*$B$3/I22/1000000</f>
+        <v>16.1977181425022</v>
+      </c>
+      <c r="J24" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="K24" s="0" t="n">
+        <f aca="false">$A$3*$B$3/K22/1000000</f>
+        <v>15.7947591361894</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:K21"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:K76"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F82" activeCellId="0" sqref="F82"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="26.1887755102041"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="28"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <f aca="false">128*128</f>
+        <v>16384</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="H4" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="D5" s="30"/>
+      <c r="H5" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="K5" s="30"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>10.24</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>10.62</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="J6" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>11.57</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>9.14</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>9.47</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>8.81</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <f aca="false">$A$3*$B$3/B6/1000000</f>
+        <v>16</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>0.014326</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="I8" s="0" t="e">
+        <f aca="false">$A$3*$B$3/I6/1000000</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J8" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>0.009981</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>1.51301</v>
+      </c>
+      <c r="H9" s="28"/>
+      <c r="J9" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>1.193948</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10" s="30"/>
+      <c r="C10" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>0.688278</v>
+      </c>
+      <c r="H10" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="I10" s="30"/>
+      <c r="J10" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>0.646576</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>11.07</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>0.287723</v>
+      </c>
+      <c r="H11" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>9.96</v>
+      </c>
+      <c r="J11" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>0.289514</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>9.99</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>1.952167</v>
+      </c>
+      <c r="H12" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="J12" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>1.809679</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <f aca="false">$A$3*$B$3/B11/1000000</f>
+        <v>14.8003613369467</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>4.443027</v>
+      </c>
+      <c r="H13" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <f aca="false">$A$3*$B$3/I11/1000000</f>
+        <v>16.4497991967871</v>
+      </c>
+      <c r="J13" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>4.333459</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="28"/>
+      <c r="J14" s="28"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="B15" s="30"/>
+      <c r="H15" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="I15" s="30"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>10.85</v>
+      </c>
+      <c r="H16" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>9.74</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>9.74</v>
+      </c>
+      <c r="H17" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>8.68</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <f aca="false">$A$3*$B$3/B16/1000000</f>
+        <v>15.1004608294931</v>
+      </c>
+      <c r="H18" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <f aca="false">$A$3*$B$3/I16/1000000</f>
+        <v>16.8213552361396</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="B20" s="30"/>
+      <c r="H20" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="I20" s="30"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>12.06</v>
+      </c>
+      <c r="H21" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>10.56</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>9.55</v>
+      </c>
+      <c r="H22" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>8.67</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <f aca="false">$A$3*$B$3/B21/1000000</f>
+        <v>13.5854063018242</v>
+      </c>
+      <c r="H23" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <f aca="false">$A$3*$B$3/I21/1000000</f>
+        <v>15.5151515151515</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="D25" s="30"/>
+      <c r="H25" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="I25" s="30"/>
+      <c r="J25" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="K25" s="30"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>10.26</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>10.74</v>
+      </c>
+      <c r="H26" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="I26" s="0" t="n">
+        <v>9.87</v>
+      </c>
+      <c r="J26" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="K26" s="0" t="n">
+        <v>9.75</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>9.3</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>2.838665</v>
+      </c>
+      <c r="H27" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <v>8.85</v>
+      </c>
+      <c r="J27" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="K27" s="0" t="n">
+        <v>2.259328</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <f aca="false">$A$3*$B$3/B26/1000000</f>
+        <v>15.9688109161793</v>
+      </c>
+      <c r="C28" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <f aca="false">$A$3*$B$3/D26/1000000</f>
+        <v>15.2551210428305</v>
+      </c>
+      <c r="H28" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="I28" s="0" t="n">
+        <f aca="false">$A$3*$B$3/I26/1000000</f>
+        <v>16.5997973657548</v>
+      </c>
+      <c r="J28" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="K28" s="0" t="n">
+        <f aca="false">$A$3*$B$3/K26/1000000</f>
+        <v>16.8041025641026</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="B31" s="28"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="28" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <f aca="false">64*64*64</f>
+        <v>262144</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="B34" s="30"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+      <c r="H34" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="I34" s="30"/>
+      <c r="J34" s="30"/>
+      <c r="K34" s="30"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="B35" s="30"/>
+      <c r="C35" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="D35" s="30"/>
+      <c r="H35" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="I35" s="30"/>
+      <c r="J35" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="K35" s="30"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="C36" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>83.7</v>
+      </c>
+      <c r="H36" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="J36" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="K36" s="0" t="n">
+        <v>50.279999</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>79.1</v>
+      </c>
+      <c r="H37" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="J37" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="K37" s="0" t="n">
+        <v>48.490002</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="B38" s="0" t="e">
+        <f aca="false">$A$33*$B$33/B36/1000000</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C38" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>0.055832</v>
+      </c>
+      <c r="H38" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="I38" s="0" t="e">
+        <f aca="false">$A$33*$B$33/I36/1000000</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J38" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="K38" s="0" t="n">
+        <v>0.052599</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C39" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>28.990219</v>
+      </c>
+      <c r="J39" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="K39" s="0" t="n">
+        <v>11.452539</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="30"/>
+      <c r="B40" s="30"/>
+      <c r="C40" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>7.859793</v>
+      </c>
+      <c r="H40" s="30"/>
+      <c r="I40" s="30"/>
+      <c r="J40" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="K40" s="0" t="n">
+        <v>4.704807</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="28"/>
+      <c r="C41" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>1.781338</v>
+      </c>
+      <c r="H41" s="28"/>
+      <c r="J41" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="K41" s="0" t="n">
+        <v>1.625322</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="28"/>
+      <c r="C42" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>15.371088</v>
+      </c>
+      <c r="H42" s="28"/>
+      <c r="J42" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="K42" s="0" t="n">
+        <v>9.340991</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="28"/>
+      <c r="C43" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>16.571722</v>
+      </c>
+      <c r="H43" s="28"/>
+      <c r="J43" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="K43" s="0" t="n">
+        <v>14.906499</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C44" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <f aca="false">$A$33*$B$33/D36/1000000</f>
+        <v>31.3194743130227</v>
+      </c>
+      <c r="J44" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="K44" s="0" t="n">
+        <f aca="false">$A$33*$B$33/K36/1000000</f>
+        <v>52.1368347680357</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="B46" s="30"/>
+      <c r="C46" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="D46" s="30"/>
+      <c r="H46" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="K46" s="30"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="H47" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="I47" s="0" t="n">
+        <v>48.540001</v>
+      </c>
+      <c r="J47" s="28" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C48" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="H48" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="I48" s="0" t="n">
+        <v>46.889999</v>
+      </c>
+      <c r="J48" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="B49" s="0" t="e">
+        <f aca="false">$A$33*$B$33/B47/1000000</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C49" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="D49" s="0" t="e">
+        <f aca="false">$A$33*$B$33/D47/1000000</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H49" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="I49" s="0" t="n">
+        <f aca="false">$A$33*$B$33/I47/1000000</f>
+        <v>54.005767325798</v>
+      </c>
+      <c r="J49" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="K49" s="0" t="e">
+        <f aca="false">$A$33*$B$33/K47/1000000</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="30"/>
+      <c r="B50" s="30"/>
+      <c r="H50" s="30"/>
+      <c r="I50" s="30"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="28"/>
+      <c r="H51" s="28"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="B52" s="28"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B53" s="28" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="n">
+        <f aca="false">128*128*128</f>
+        <v>2097152</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="B55" s="30"/>
+      <c r="C55" s="30"/>
+      <c r="D55" s="30"/>
+      <c r="H55" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="I55" s="30"/>
+      <c r="J55" s="30"/>
+      <c r="K55" s="30"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="B56" s="30"/>
+      <c r="C56" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="D56" s="30"/>
+      <c r="H56" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="I56" s="30"/>
+      <c r="J56" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="K56" s="30"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="C57" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>469.29</v>
+      </c>
+      <c r="H57" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="J57" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="K57" s="0" t="n">
+        <v>265.040009</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C58" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <v>457.81</v>
+      </c>
+      <c r="H58" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="J58" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="K58" s="0" t="n">
+        <v>253.580002</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="B59" s="0" t="e">
+        <f aca="false">$A$54*$B$54/B57/1000000</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C59" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <v>0.378547</v>
+      </c>
+      <c r="H59" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="I59" s="0" t="e">
+        <f aca="false">$A$33*$B$33/I57/1000000</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J59" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="K59" s="0" t="n">
+        <v>0.336721</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C60" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D60" s="0" t="n">
+        <v>171.481796</v>
+      </c>
+      <c r="J60" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="K60" s="0" t="n">
+        <v>76.123222</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="30"/>
+      <c r="B61" s="30"/>
+      <c r="C61" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D61" s="0" t="n">
+        <v>62.200644</v>
+      </c>
+      <c r="H61" s="30"/>
+      <c r="I61" s="30"/>
+      <c r="J61" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="K61" s="0" t="n">
+        <v>36.679489</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="28"/>
+      <c r="C62" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62" s="0" t="n">
+        <v>6.354612</v>
+      </c>
+      <c r="H62" s="28"/>
+      <c r="J62" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="K62" s="0" t="n">
+        <v>5.879762</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="28"/>
+      <c r="C63" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" s="0" t="n">
+        <v>110.044451</v>
+      </c>
+      <c r="H63" s="28"/>
+      <c r="J63" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="K63" s="0" t="n">
+        <v>64.443375</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="28"/>
+      <c r="C64" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D64" s="0" t="n">
+        <v>69.055508</v>
+      </c>
+      <c r="H64" s="28"/>
+      <c r="J64" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="K64" s="0" t="n">
+        <v>49.072239</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C65" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="D65" s="0" t="n">
+        <f aca="false">$A$54*$B$54/D57/1000000</f>
+        <v>44.6877623644229</v>
+      </c>
+      <c r="J65" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="K65" s="0" t="n">
+        <f aca="false">$A$54*$B$54/K57/1000000</f>
+        <v>79.1258651066526</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="B67" s="30"/>
+      <c r="C67" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="D67" s="30"/>
+      <c r="H67" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="I67" s="30"/>
+      <c r="J67" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="K67" s="30"/>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B68" s="0" t="n">
+        <v>473.89</v>
+      </c>
+      <c r="C68" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="H68" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="I68" s="0" t="n">
+        <v>257.029999</v>
+      </c>
+      <c r="J68" s="28" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B69" s="0" t="n">
+        <v>462.57</v>
+      </c>
+      <c r="C69" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="H69" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="I69" s="0" t="n">
+        <v>245.539993</v>
+      </c>
+      <c r="J69" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B70" s="0" t="n">
+        <v>0.379627</v>
+      </c>
+      <c r="C70" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="D70" s="0" t="e">
+        <f aca="false">$A$54*$B$54/D68/1000000</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H70" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="I70" s="0" t="n">
+        <v>0.315908</v>
+      </c>
+      <c r="J70" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="K70" s="0" t="e">
+        <f aca="false">$A$54*$B$54/K68/1000000</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B71" s="0" t="n">
+        <v>176.84227</v>
+      </c>
+      <c r="H71" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="I71" s="0" t="n">
+        <v>75.413963</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B72" s="0" t="n">
+        <v>62.168519</v>
+      </c>
+      <c r="H72" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="I72" s="0" t="n">
+        <v>36.413788</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B73" s="0" t="n">
+        <v>6.460029</v>
+      </c>
+      <c r="H73" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="I73" s="0" t="n">
+        <v>5.83298</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B74" s="0" t="n">
+        <v>109.94352</v>
+      </c>
+      <c r="H74" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="I74" s="0" t="n">
+        <v>63.839321</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B75" s="0" t="n">
+        <v>68.804625</v>
+      </c>
+      <c r="H75" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="I75" s="0" t="n">
+        <v>44.465824</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="B76" s="0" t="n">
+        <f aca="false">$A$54*$B$54/B68/1000000</f>
+        <v>44.2539829918336</v>
+      </c>
+      <c r="H76" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="I76" s="0" t="n">
+        <f aca="false">$A$54*$B$54/I68/1000000</f>
+        <v>81.5917211282408</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="42">
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="H34:K34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="H55:K55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="J56:K56"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="H67:I67"/>
+    <mergeCell ref="J67:K67"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
ready to start discussing performance
</commit_message>
<xml_diff>
--- a/Thesis/Resources/CGPerformance.xlsx
+++ b/Thesis/Resources/CGPerformance.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -444,12 +444,11 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -471,16 +470,10 @@
       <color rgb="FF000000"/>
       <name val="Monospace"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="13"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -501,21 +494,18 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF212121"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -742,111 +732,107 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -854,7 +840,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -862,7 +852,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1330,11 +1320,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="58512202"/>
-        <c:axId val="39121084"/>
+        <c:axId val="23272102"/>
+        <c:axId val="48244195"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="58512202"/>
+        <c:axId val="23272102"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1378,14 +1368,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39121084"/>
+        <c:crossAx val="48244195"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39121084"/>
+        <c:axId val="48244195"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1476,7 +1466,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58512202"/>
+        <c:crossAx val="23272102"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1654,11 +1644,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="60212111"/>
-        <c:axId val="97322992"/>
+        <c:axId val="67113265"/>
+        <c:axId val="98918835"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="60212111"/>
+        <c:axId val="67113265"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1693,14 +1683,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97322992"/>
+        <c:crossAx val="98918835"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97322992"/>
+        <c:axId val="98918835"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1782,7 +1772,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60212111"/>
+        <c:crossAx val="67113265"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1869,10 +1859,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.194767932489451"/>
-          <c:y val="0.14704901633878"/>
-          <c:w val="0.531898734177215"/>
-          <c:h val="0.829276425475158"/>
+          <c:x val="0.19471834004973"/>
+          <c:y val="0.147065362383281"/>
+          <c:w val="0.531852868044243"/>
+          <c:h val="0.829146287238773"/>
         </c:manualLayout>
       </c:layout>
       <c:pieChart>
@@ -2222,11 +2212,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="24343379"/>
-        <c:axId val="78668940"/>
+        <c:axId val="55359946"/>
+        <c:axId val="51244380"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="24343379"/>
+        <c:axId val="55359946"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2261,14 +2251,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78668940"/>
+        <c:crossAx val="51244380"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78668940"/>
+        <c:axId val="51244380"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2350,7 +2340,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="24343379"/>
+        <c:crossAx val="55359946"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2392,15 +2382,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>524520</xdr:colOff>
+      <xdr:colOff>525240</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>124560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>437400</xdr:colOff>
+      <xdr:colOff>437040</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>94680</xdr:rowOff>
+      <xdr:rowOff>94320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2408,8 +2398,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6915600" y="124560"/>
-        <a:ext cx="5389920" cy="3221280"/>
+        <a:off x="6820920" y="124560"/>
+        <a:ext cx="5303160" cy="3220920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2424,13 +2414,13 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>441360</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>2880</xdr:rowOff>
+      <xdr:rowOff>3600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1226880</xdr:colOff>
+      <xdr:colOff>1227240</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>150120</xdr:rowOff>
+      <xdr:rowOff>149760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2438,8 +2428,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5632200" y="4879440"/>
-        <a:ext cx="4138560" cy="3236040"/>
+        <a:off x="5556240" y="4880160"/>
+        <a:ext cx="4081320" cy="3234960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2452,15 +2442,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>512280</xdr:colOff>
+      <xdr:colOff>513000</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>86400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>337320</xdr:colOff>
+      <xdr:colOff>336960</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>74160</xdr:rowOff>
+      <xdr:rowOff>73800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2468,8 +2458,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7913160" y="8376840"/>
-        <a:ext cx="4292280" cy="3238920"/>
+        <a:off x="7799400" y="8376840"/>
+        <a:ext cx="4224600" cy="3238560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2482,15 +2472,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>132840</xdr:colOff>
+      <xdr:colOff>133560</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>117720</xdr:rowOff>
+      <xdr:rowOff>118440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>197640</xdr:colOff>
+      <xdr:colOff>198000</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>105120</xdr:rowOff>
+      <xdr:rowOff>105480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2498,8 +2488,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="12600720" y="280080"/>
-        <a:ext cx="4265640" cy="3238560"/>
+        <a:off x="12411000" y="280800"/>
+        <a:ext cx="4198320" cy="3238200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2512,15 +2502,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>74880</xdr:colOff>
+      <xdr:colOff>75600</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>28800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>690480</xdr:colOff>
+      <xdr:colOff>690840</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>16560</xdr:rowOff>
+      <xdr:rowOff>16200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2528,8 +2518,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3465720" y="8319240"/>
-        <a:ext cx="3615840" cy="3238920"/>
+        <a:off x="3418560" y="8319240"/>
+        <a:ext cx="3567960" cy="3238560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2555,16 +2545,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="9" min="5" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="9" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3345,17 +3335,17 @@
   </sheetPr>
   <dimension ref="A1:W54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="V54" activeCellId="0" sqref="V54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="9" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.5204081632653"/>
-    <col collapsed="false" hidden="false" max="20" min="11" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="12.8061224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="20" min="11" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5420,13 +5410,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5643,20 +5636,22 @@
   </sheetPr>
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H22" activeCellId="0" sqref="H22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6101,20 +6096,22 @@
   </sheetPr>
   <dimension ref="A1:K76"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F82" activeCellId="0" sqref="F82"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I47" activeCellId="0" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="26.1887755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.7857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>